<commit_message>
UC 1 - Test Scenarios
</commit_message>
<xml_diff>
--- a/Análise/Test Scenarios.xlsx
+++ b/Análise/Test Scenarios.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\upskill_java1_labprg_grupo3\Análise\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BAA3D0-09AE-42CF-B41C-F5D4EB3B510A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Mover ficheiro" sheetId="2" r:id="rId2"/>
-    <sheet name="Cancelar encomenda" sheetId="3" r:id="rId3"/>
+    <sheet name="UC 1 - Registar Organização" sheetId="7" r:id="rId3"/>
     <sheet name="UC 4 - Definir Comp.Técnica" sheetId="4" r:id="rId4"/>
     <sheet name="UC 5 - Especificar Colab.Org" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="79">
   <si>
     <t>Project Name</t>
   </si>
@@ -250,22 +256,56 @@
     <t>Falha</t>
   </si>
   <si>
-    <t>Cancelar encomenda que já foi cancelada</t>
-  </si>
-  <si>
-    <t>Cancelar encomenda que existe e não foi ainda cncelada</t>
-  </si>
-  <si>
-    <t>Cancelar encomenda que não existe</t>
-  </si>
-  <si>
-    <t>Cancelar encomenda que não é reembolsável</t>
+    <t>Check Registar Organização functionality</t>
+  </si>
+  <si>
+    <t>TC_UC1_001</t>
+  </si>
+  <si>
+    <t>TC_UC1_002</t>
+  </si>
+  <si>
+    <t>TC_UC1_003</t>
+  </si>
+  <si>
+    <t>TC_UC1_004</t>
+  </si>
+  <si>
+    <t>Valid Org Name
+Valid Org NIF
+Valid Org Email
+Valid Org Website
+Valid Org Phone Number
+Valid Org Address</t>
+  </si>
+  <si>
+    <t>1. Enter valid org name
+2. Enter valid org nif
+3. Enter valid org email
+4. Enter valid org website
+5. Enter valid org phone number
+6. Enter valid org address
+7. Click register button</t>
+  </si>
+  <si>
+    <t>org name: org123
+org nif: 123456789
+org email: org123@org123.com
+org website: org123.com
+org phone number: 911123123
+org address: rua sousa, 1, 4000-400, Porto</t>
+  </si>
+  <si>
+    <t>Message "Organization successfully registered"</t>
+  </si>
+  <si>
+    <t>Successful register of an Organization</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -344,8 +384,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Texto Explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -421,12 +461,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -468,7 +511,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,9 +544,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,6 +596,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -711,7 +788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -960,11 +1037,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1209,19 +1286,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B64CDF4-CC92-40F1-801A-4C473A6BB3C1}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.75"/>
-    <col min="2" max="2" width="24" style="1"/>
-    <col min="3" max="5" width="24"/>
-    <col min="6" max="1025" width="10.875"/>
+    <col min="1" max="1" width="25.25" customWidth="1"/>
+    <col min="2" max="2" width="25.25" style="1" customWidth="1"/>
+    <col min="3" max="5" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1277,7 +1353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1285,83 +1361,156 @@
         <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="126" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B17"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -1385,7 +1534,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1397,10 +1546,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>